<commit_message>
fix waiting time and avg rate
</commit_message>
<xml_diff>
--- a/src/gatourism/data_P_fix.xlsx
+++ b/src/gatourism/data_P_fix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\Tourism\Tourism\src\gatourism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E64450F-BBF6-4A4E-9D8F-1D737D878053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071C434D-54F2-47B0-9583-4366A38B235F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="N178" sqref="N178"/>
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>82800</v>
       </c>
       <c r="E65" s="14">
-        <v>0</v>
+        <v>150000</v>
       </c>
       <c r="F65" s="11">
         <f t="shared" si="0"/>
@@ -2607,7 +2607,7 @@
         <v>82800</v>
       </c>
       <c r="E66" s="14">
-        <v>0</v>
+        <v>245000</v>
       </c>
       <c r="F66" s="11">
         <f t="shared" si="0"/>
@@ -2631,7 +2631,7 @@
         <v>79200</v>
       </c>
       <c r="E67" s="14">
-        <v>0</v>
+        <v>810000</v>
       </c>
       <c r="F67" s="11">
         <f t="shared" ref="F67:F130" si="1">3600*G67</f>
@@ -2655,7 +2655,7 @@
         <v>79200</v>
       </c>
       <c r="E68" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F68" s="11">
         <f t="shared" si="1"/>
@@ -2679,7 +2679,7 @@
         <v>81000</v>
       </c>
       <c r="E69" s="14">
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="F69" s="11">
         <f t="shared" si="1"/>
@@ -2703,7 +2703,7 @@
         <v>82800</v>
       </c>
       <c r="E70" s="14">
-        <v>0</v>
+        <v>240000</v>
       </c>
       <c r="F70" s="11">
         <f t="shared" si="1"/>
@@ -2713,7 +2713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>72000</v>
       </c>
       <c r="E72" s="14">
-        <v>0</v>
+        <v>390000</v>
       </c>
       <c r="F72" s="11">
         <f t="shared" si="1"/>
@@ -2775,7 +2775,7 @@
         <v>79200</v>
       </c>
       <c r="E73" s="14">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="F73" s="11">
         <f t="shared" si="1"/>
@@ -2799,7 +2799,7 @@
         <v>86160</v>
       </c>
       <c r="E74" s="14">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="F74" s="11">
         <f t="shared" si="1"/>
@@ -2823,7 +2823,7 @@
         <v>77400</v>
       </c>
       <c r="E75" s="14">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="F75" s="11">
         <f t="shared" si="1"/>
@@ -2871,7 +2871,7 @@
         <v>43200</v>
       </c>
       <c r="E77" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F77" s="11">
         <f t="shared" si="1"/>
@@ -2895,7 +2895,7 @@
         <v>75600</v>
       </c>
       <c r="E78" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F78" s="11">
         <f t="shared" si="1"/>
@@ -2919,7 +2919,7 @@
         <v>68400</v>
       </c>
       <c r="E79" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F79" s="11">
         <f t="shared" si="1"/>
@@ -2991,7 +2991,7 @@
         <v>84600</v>
       </c>
       <c r="E82" s="14">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="F82" s="11">
         <f t="shared" si="1"/>
@@ -3015,7 +3015,7 @@
         <v>82800</v>
       </c>
       <c r="E83" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F83" s="11">
         <f t="shared" si="1"/>
@@ -3039,7 +3039,7 @@
         <v>79200</v>
       </c>
       <c r="E84" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F84" s="11">
         <f t="shared" si="1"/>
@@ -3062,9 +3062,7 @@
       <c r="D85">
         <v>84600</v>
       </c>
-      <c r="E85" s="14">
-        <v>0</v>
-      </c>
+      <c r="E85" s="14"/>
       <c r="F85" s="11">
         <f t="shared" si="1"/>
         <v>7200</v>
@@ -3087,7 +3085,7 @@
         <v>81000</v>
       </c>
       <c r="E86" s="14">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="F86" s="11">
         <f t="shared" si="1"/>
@@ -3111,7 +3109,7 @@
         <v>81000</v>
       </c>
       <c r="E87" s="14">
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="F87" s="11">
         <f t="shared" si="1"/>
@@ -3135,7 +3133,7 @@
         <v>84600</v>
       </c>
       <c r="E88" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F88" s="11">
         <f t="shared" si="1"/>
@@ -3159,7 +3157,7 @@
         <v>68400</v>
       </c>
       <c r="E89" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F89" s="11">
         <f t="shared" si="1"/>
@@ -3183,7 +3181,7 @@
         <v>84600</v>
       </c>
       <c r="E90" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F90" s="11">
         <f t="shared" si="1"/>
@@ -3207,7 +3205,7 @@
         <v>68400</v>
       </c>
       <c r="E91" s="14">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="F91" s="11">
         <f t="shared" si="1"/>
@@ -3231,7 +3229,7 @@
         <v>84600</v>
       </c>
       <c r="E92" s="14">
-        <v>0</v>
+        <v>480000</v>
       </c>
       <c r="F92" s="11">
         <f t="shared" si="1"/>
@@ -3255,7 +3253,7 @@
         <v>75600</v>
       </c>
       <c r="E93" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F93" s="11">
         <f t="shared" si="1"/>
@@ -3303,7 +3301,7 @@
         <v>79200</v>
       </c>
       <c r="E95" s="14">
-        <v>0</v>
+        <v>140000</v>
       </c>
       <c r="F95" s="11">
         <f t="shared" si="1"/>
@@ -3327,7 +3325,7 @@
         <v>79200</v>
       </c>
       <c r="E96" s="14">
-        <v>0</v>
+        <v>450000</v>
       </c>
       <c r="F96" s="11">
         <f t="shared" si="1"/>
@@ -3351,7 +3349,7 @@
         <v>72000</v>
       </c>
       <c r="E97" s="14">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F97" s="11">
         <f t="shared" si="1"/>
@@ -3375,7 +3373,7 @@
         <v>75600</v>
       </c>
       <c r="E98" s="14">
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="F98" s="11">
         <f t="shared" si="1"/>
@@ -3399,7 +3397,7 @@
         <v>7200</v>
       </c>
       <c r="E99" s="14">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="F99" s="11">
         <f t="shared" si="1"/>
@@ -3423,7 +3421,7 @@
         <v>79200</v>
       </c>
       <c r="E100" s="14">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="F100" s="11">
         <f t="shared" si="1"/>
@@ -3447,7 +3445,7 @@
         <v>72000</v>
       </c>
       <c r="E101" s="14">
-        <v>0</v>
+        <v>800000</v>
       </c>
       <c r="F101" s="11">
         <f t="shared" si="1"/>
@@ -3495,7 +3493,7 @@
         <v>79200</v>
       </c>
       <c r="E103" s="14">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="F103" s="11">
         <f t="shared" si="1"/>
@@ -3519,7 +3517,7 @@
         <v>72000</v>
       </c>
       <c r="E104" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F104" s="11">
         <f t="shared" si="1"/>
@@ -3543,7 +3541,7 @@
         <v>43200</v>
       </c>
       <c r="E105" s="14">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="F105" s="11">
         <f t="shared" si="1"/>
@@ -3601,7 +3599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>

</xml_diff>